<commit_message>
Updating data from task 2, 3, and 4
</commit_message>
<xml_diff>
--- a/homework/hw3/HW3_data.xlsx
+++ b/homework/hw3/HW3_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b1fe7c3d1cebb12/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clari\OneDrive\Documents\math5620\homework\hw3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2DF1757-AE39-4848-BDA0-01944F123474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{E2DF1757-AE39-4848-BDA0-01944F123474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{918D8B0E-3C3A-430A-BBC9-64458AED3F68}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{1157FCA2-EFAF-4B11-9037-E5F838C48317}"/>
   </bookViews>
@@ -13150,16 +13150,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>87075</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>107056</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>361836</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>52104</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>577565</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>109113</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>202062</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>54161</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13186,16 +13186,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>185207</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>44098</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>414174</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>99051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>31877</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>46157</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>260843</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>101109</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13224,16 +13224,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>105835</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>52915</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>398914</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>126184</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>598089</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>54974</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>240904</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>128242</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13562,8 +13562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03D5126-57C5-41D7-BA37-1C698C0B9448}">
   <dimension ref="A1:Y259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="67" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="99" workbookViewId="0">
+      <selection activeCell="AK62" sqref="AK62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -13573,7 +13573,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="H1" t="s">
         <v>0</v>
       </c>
       <c r="N1" t="s">

</xml_diff>